<commit_message>
Add cities + Grafic test
</commit_message>
<xml_diff>
--- a/Monitoramento_Clima.xlsx
+++ b/Monitoramento_Clima.xlsx
@@ -8,18 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\Data_Science_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC84EFA-A465-4AC7-95E5-1BEB8CED4D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F65D20E-DB40-4FEB-B0FB-EF7D1B0C8767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela_Clima" sheetId="1" r:id="rId1"/>
-    <sheet name="Relatório" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelas dinâmicas" sheetId="4" r:id="rId2"/>
+    <sheet name="Relatório" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="7" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Data</t>
   </si>
@@ -75,11 +79,35 @@
   <si>
     <t>Velocidade do vento</t>
   </si>
+  <si>
+    <t>Rótulos de Linha</t>
+  </si>
+  <si>
+    <t>Acaraú</t>
+  </si>
+  <si>
+    <t>Fortaleza</t>
+  </si>
+  <si>
+    <t>Itarema</t>
+  </si>
+  <si>
+    <t>Sobral</t>
+  </si>
+  <si>
+    <t>Total Geral</t>
+  </si>
+  <si>
+    <t>Média de Teperatura</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.00\°"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,22 +137,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="27">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00\°"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\º"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -133,9 +209,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -181,6 +254,1239 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Monitoramento_Clima.xlsx]Tabelas dinâmicas!Tabela dinâmica2</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="002060"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1800" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="002060"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Temperaturas</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1800" b="1" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="002060"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Médias por Cidade</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="002060"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="40000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tabelas dinâmicas'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:prstClr val="black">
+                  <a:alpha val="40000"/>
+                </a:prstClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-F3E5-49BD-A8D1-ADD80254710E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F3E5-49BD-A8D1-ADD80254710E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-F3E5-49BD-A8D1-ADD80254710E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F3E5-49BD-A8D1-ADD80254710E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Tabelas dinâmicas'!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Acaraú</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fortaleza</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Itarema</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sobral</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tabelas dinâmicas'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00\°</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>30.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.71</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F3E5-49BD-A8D1-ADD80254710E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="70"/>
+        <c:overlap val="-27"/>
+        <c:axId val="496838304"/>
+        <c:axId val="496836640"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="496838304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="496836640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="496836640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00\°" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="496838304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42204347-5169-4014-82C3-6219F74636E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -190,44 +1496,155 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
-          <cell r="A2">
-            <v>0</v>
-          </cell>
           <cell r="B2" t="str">
-            <v>25\08\24</v>
+            <v>09\09\24</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Dom</v>
+            <v>seg</v>
           </cell>
           <cell r="D2" t="str">
-            <v>12:33:00</v>
+            <v>14:27:06</v>
           </cell>
           <cell r="E2" t="str">
-            <v>Itarema</v>
+            <v>Fortaleza</v>
           </cell>
           <cell r="F2" t="str">
-            <v>céu limpo</v>
+            <v>algumas nuvens</v>
           </cell>
           <cell r="G2">
-            <v>25</v>
+            <v>31.71</v>
           </cell>
           <cell r="H2">
-            <v>25</v>
+            <v>31.07</v>
           </cell>
           <cell r="I2">
-            <v>25</v>
+            <v>31.71</v>
           </cell>
           <cell r="J2">
-            <v>25.3</v>
+            <v>38.71</v>
           </cell>
           <cell r="K2">
-            <v>70</v>
+            <v>83</v>
           </cell>
           <cell r="L2">
             <v>1013</v>
           </cell>
           <cell r="M2">
-            <v>7</v>
+            <v>9.77</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>09\09\24</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>seg</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>14:27:06</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>Sobral</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>céu limpo</v>
+          </cell>
+          <cell r="G3">
+            <v>36.28</v>
+          </cell>
+          <cell r="H3">
+            <v>36.28</v>
+          </cell>
+          <cell r="I3">
+            <v>36.28</v>
+          </cell>
+          <cell r="J3">
+            <v>34.68</v>
+          </cell>
+          <cell r="K3">
+            <v>21</v>
+          </cell>
+          <cell r="L3">
+            <v>1011</v>
+          </cell>
+          <cell r="M3">
+            <v>3.85</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>09\09\24</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>seg</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>14:27:06</v>
+          </cell>
+          <cell r="E4" t="str">
+            <v>Acaraú</v>
+          </cell>
+          <cell r="F4" t="str">
+            <v>céu limpo</v>
+          </cell>
+          <cell r="G4">
+            <v>30.77</v>
+          </cell>
+          <cell r="H4">
+            <v>30.77</v>
+          </cell>
+          <cell r="I4">
+            <v>30.77</v>
+          </cell>
+          <cell r="J4">
+            <v>32.43</v>
+          </cell>
+          <cell r="K4">
+            <v>51</v>
+          </cell>
+          <cell r="L4">
+            <v>1011</v>
+          </cell>
+          <cell r="M4">
+            <v>10.02</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>09\09\24</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>seg</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>14:27:06</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>Itarema</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>céu limpo</v>
+          </cell>
+          <cell r="G5">
+            <v>29.93</v>
+          </cell>
+          <cell r="H5">
+            <v>29.93</v>
+          </cell>
+          <cell r="I5">
+            <v>29.93</v>
+          </cell>
+          <cell r="J5">
+            <v>31.26</v>
+          </cell>
+          <cell r="K5">
+            <v>52</v>
+          </cell>
+          <cell r="L5">
+            <v>1012</v>
+          </cell>
+          <cell r="M5">
+            <v>9.6999999999999993</v>
           </cell>
         </row>
       </sheetData>
@@ -236,45 +1653,345 @@
 </externalLink>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Gabriel" refreshedDate="45544.616618865737" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="8" xr:uid="{85AEFC04-348E-4CC1-A114-5BCE553812B3}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Monitoramento_Clima"/>
+  </cacheSource>
+  <cacheFields count="12">
+    <cacheField name="Data" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Dia da semana" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Hora" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Cidade" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Fortaleza"/>
+        <s v="Sobral"/>
+        <s v="Acaraú"/>
+        <s v="Itarema"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Status" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Teperatura" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="29.93" maxValue="36.28"/>
+    </cacheField>
+    <cacheField name="Temperatura mínima" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="29.93" maxValue="36.28"/>
+    </cacheField>
+    <cacheField name="Temperatura máxima" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="29.93" maxValue="36.28"/>
+    </cacheField>
+    <cacheField name="Sensação térmica" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="31.26" maxValue="38.71"/>
+    </cacheField>
+    <cacheField name="Humidade do ar" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="21" maxValue="83"/>
+    </cacheField>
+    <cacheField name="Pressão atmosférica" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1011" maxValue="1013"/>
+    </cacheField>
+    <cacheField name="Velocidade do vento" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.85" maxValue="10.02"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="8">
+  <r>
+    <s v="09\09\24"/>
+    <s v="seg"/>
+    <s v="14:27:06"/>
+    <x v="0"/>
+    <s v="algumas nuvens"/>
+    <n v="31.71"/>
+    <n v="31.07"/>
+    <n v="31.71"/>
+    <n v="38.71"/>
+    <n v="83"/>
+    <n v="1013"/>
+    <n v="9.77"/>
+  </r>
+  <r>
+    <s v="09\09\24"/>
+    <s v="seg"/>
+    <s v="14:27:06"/>
+    <x v="1"/>
+    <s v="céu limpo"/>
+    <n v="36.28"/>
+    <n v="36.28"/>
+    <n v="36.28"/>
+    <n v="34.68"/>
+    <n v="21"/>
+    <n v="1011"/>
+    <n v="3.85"/>
+  </r>
+  <r>
+    <s v="09\09\24"/>
+    <s v="seg"/>
+    <s v="14:27:06"/>
+    <x v="2"/>
+    <s v="céu limpo"/>
+    <n v="30.77"/>
+    <n v="30.77"/>
+    <n v="30.77"/>
+    <n v="32.43"/>
+    <n v="51"/>
+    <n v="1011"/>
+    <n v="10.02"/>
+  </r>
+  <r>
+    <s v="09\09\24"/>
+    <s v="seg"/>
+    <s v="14:27:06"/>
+    <x v="3"/>
+    <s v="céu limpo"/>
+    <n v="29.93"/>
+    <n v="29.93"/>
+    <n v="29.93"/>
+    <n v="31.26"/>
+    <n v="52"/>
+    <n v="1012"/>
+    <n v="9.6999999999999993"/>
+  </r>
+  <r>
+    <s v="09\09\24"/>
+    <s v="seg"/>
+    <s v="14:28:20"/>
+    <x v="0"/>
+    <s v="algumas nuvens"/>
+    <n v="31.71"/>
+    <n v="31.07"/>
+    <n v="31.71"/>
+    <n v="38.71"/>
+    <n v="83"/>
+    <n v="1013"/>
+    <n v="9.77"/>
+  </r>
+  <r>
+    <s v="09\09\24"/>
+    <s v="seg"/>
+    <s v="14:28:20"/>
+    <x v="1"/>
+    <s v="céu limpo"/>
+    <n v="36.28"/>
+    <n v="36.28"/>
+    <n v="36.28"/>
+    <n v="34.68"/>
+    <n v="21"/>
+    <n v="1011"/>
+    <n v="3.85"/>
+  </r>
+  <r>
+    <s v="09\09\24"/>
+    <s v="seg"/>
+    <s v="14:28:20"/>
+    <x v="2"/>
+    <s v="céu limpo"/>
+    <n v="30.77"/>
+    <n v="30.77"/>
+    <n v="30.77"/>
+    <n v="32.43"/>
+    <n v="51"/>
+    <n v="1011"/>
+    <n v="10.02"/>
+  </r>
+  <r>
+    <s v="09\09\24"/>
+    <s v="seg"/>
+    <s v="14:28:20"/>
+    <x v="3"/>
+    <s v="céu limpo"/>
+    <n v="29.93"/>
+    <n v="29.93"/>
+    <n v="29.93"/>
+    <n v="31.26"/>
+    <n v="52"/>
+    <n v="1012"/>
+    <n v="9.6999999999999993"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B2DF444-137A-4B80-9AD3-D03A104B5F35}" name="Tabela dinâmica2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A1:B6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Média de Teperatura" fld="5" subtotal="average" baseField="0" baseItem="0" numFmtId="167"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="5">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96DEBF73-C1B5-4AF8-883C-AA81214D6D4F}" name="Monitoramento_Clima" displayName="Monitoramento_Clima" ref="A1:L2" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L2" xr:uid="{96DEBF73-C1B5-4AF8-883C-AA81214D6D4F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96DEBF73-C1B5-4AF8-883C-AA81214D6D4F}" name="Monitoramento_Clima" displayName="Monitoramento_Clima" ref="A1:L5" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A1:L5" xr:uid="{96DEBF73-C1B5-4AF8-883C-AA81214D6D4F}"/>
   <tableColumns count="12">
-    <tableColumn id="10" xr3:uid="{033688FD-0C1C-41EF-A061-CFDD0FCDBDDC}" name="Data" dataDxfId="11">
-      <calculatedColumnFormula>[1]Sheet1!$B$2</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{033688FD-0C1C-41EF-A061-CFDD0FCDBDDC}" name="Data" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="2">
+      <calculatedColumnFormula>[1]Sheet1!B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{8BFBA493-29F8-4248-9B2A-1D7972C4CE2C}" name="Dia da semana" dataDxfId="10">
-      <calculatedColumnFormula>[1]Sheet1!$C2</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{8BFBA493-29F8-4248-9B2A-1D7972C4CE2C}" name="Dia da semana" dataDxfId="23" totalsRowDxfId="3">
+      <calculatedColumnFormula>[1]Sheet1!C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A15600C6-48FD-4906-9570-E4B2324E0708}" name="Hora" dataDxfId="9">
-      <calculatedColumnFormula>[1]Sheet1!$D2</calculatedColumnFormula>
+    <tableColumn id="12" xr3:uid="{A15600C6-48FD-4906-9570-E4B2324E0708}" name="Hora" dataDxfId="22" totalsRowDxfId="4">
+      <calculatedColumnFormula>[1]Sheet1!D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{CFA9AA23-C1BD-4634-8C59-6CF5B14F8A23}" name="Cidade" dataDxfId="8">
-      <calculatedColumnFormula>[1]Sheet1!$E2</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{CFA9AA23-C1BD-4634-8C59-6CF5B14F8A23}" name="Cidade" dataDxfId="21" totalsRowDxfId="5">
+      <calculatedColumnFormula>[1]Sheet1!E2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9942AE86-32FE-4650-80A1-1C98AD697DF8}" name="Status" dataDxfId="7">
-      <calculatedColumnFormula>[1]Sheet1!$F2</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{9942AE86-32FE-4650-80A1-1C98AD697DF8}" name="Status" dataDxfId="20" totalsRowDxfId="6">
+      <calculatedColumnFormula>[1]Sheet1!F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9C52E714-8B46-4CA1-8D21-8408F98CD104}" name="Teperatura" dataDxfId="6">
-      <calculatedColumnFormula>[1]Sheet1!$G2</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{9C52E714-8B46-4CA1-8D21-8408F98CD104}" name="Teperatura" dataDxfId="1" totalsRowDxfId="7">
+      <calculatedColumnFormula>[1]Sheet1!G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BD30C819-EE16-4F04-A7D4-A31BA8ECA99D}" name="Temperatura mínima" dataDxfId="5">
-      <calculatedColumnFormula>[1]Sheet1!$H2</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{BD30C819-EE16-4F04-A7D4-A31BA8ECA99D}" name="Temperatura mínima" dataDxfId="19" totalsRowDxfId="8">
+      <calculatedColumnFormula>[1]Sheet1!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F457E75B-7E22-4F5A-B889-ECDBCE671C10}" name="Temperatura máxima" dataDxfId="4">
-      <calculatedColumnFormula>[1]Sheet1!$I2</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{F457E75B-7E22-4F5A-B889-ECDBCE671C10}" name="Temperatura máxima" dataDxfId="18" totalsRowDxfId="9">
+      <calculatedColumnFormula>[1]Sheet1!I2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F231AEB8-BEC2-4392-A0F8-4BDB6328B880}" name="Sensação térmica" dataDxfId="3">
-      <calculatedColumnFormula>[1]Sheet1!$J2</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{F231AEB8-BEC2-4392-A0F8-4BDB6328B880}" name="Sensação térmica" dataDxfId="17" totalsRowDxfId="10">
+      <calculatedColumnFormula>[1]Sheet1!J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0DA04565-A2C1-490A-9227-3C8D24B8A4E4}" name="Humidade do ar" dataDxfId="2">
-      <calculatedColumnFormula>[1]Sheet1!$K2</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{0DA04565-A2C1-490A-9227-3C8D24B8A4E4}" name="Humidade do ar" dataDxfId="16" totalsRowDxfId="11">
+      <calculatedColumnFormula>[1]Sheet1!K2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{31A47152-D754-4B9E-AE2A-D37A5F37EF8E}" name="Pressão atmosférica" dataDxfId="1">
-      <calculatedColumnFormula>[1]Sheet1!$L2</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{31A47152-D754-4B9E-AE2A-D37A5F37EF8E}" name="Pressão atmosférica" dataDxfId="15" totalsRowDxfId="12">
+      <calculatedColumnFormula>[1]Sheet1!L2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B84CBABB-610C-4418-8E36-DBA6E84EA6E9}" name="Velocidade do vento" dataDxfId="0">
-      <calculatedColumnFormula>[1]Sheet1!$M2</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{B84CBABB-610C-4418-8E36-DBA6E84EA6E9}" name="Velocidade do vento" dataDxfId="14" totalsRowDxfId="13">
+      <calculatedColumnFormula>[1]Sheet1!M2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -547,7 +2264,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +2273,7 @@
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
@@ -606,95 +2323,203 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f>[1]Sheet1!$B2</f>
-        <v>25\08\24</v>
+        <f>[1]Sheet1!B2</f>
+        <v>09\09\24</v>
       </c>
       <c r="B2" s="1" t="str">
-        <f>[1]Sheet1!$C2</f>
-        <v>Dom</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f>[1]Sheet1!$D2</f>
-        <v>12:33:00</v>
+        <f>[1]Sheet1!C2</f>
+        <v>seg</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>[1]Sheet1!D2</f>
+        <v>14:27:06</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f>[1]Sheet1!$E2</f>
-        <v>Itarema</v>
+        <f>[1]Sheet1!E2</f>
+        <v>Fortaleza</v>
       </c>
       <c r="E2" s="1" t="str">
-        <f>[1]Sheet1!$F2</f>
-        <v>céu limpo</v>
-      </c>
-      <c r="F2" s="1">
-        <f>[1]Sheet1!$G2</f>
-        <v>25</v>
-      </c>
-      <c r="G2" s="1">
-        <f>[1]Sheet1!$H2</f>
-        <v>25</v>
-      </c>
-      <c r="H2" s="1">
-        <f>[1]Sheet1!$I2</f>
-        <v>25</v>
-      </c>
-      <c r="I2" s="1">
-        <f>[1]Sheet1!$J2</f>
-        <v>25.3</v>
-      </c>
-      <c r="J2" s="3">
-        <f>[1]Sheet1!$K2</f>
-        <v>70</v>
+        <f>[1]Sheet1!F2</f>
+        <v>algumas nuvens</v>
+      </c>
+      <c r="F2" s="5">
+        <f>[1]Sheet1!G2</f>
+        <v>31.71</v>
+      </c>
+      <c r="G2" s="5">
+        <f>[1]Sheet1!H2</f>
+        <v>31.07</v>
+      </c>
+      <c r="H2" s="5">
+        <f>[1]Sheet1!I2</f>
+        <v>31.71</v>
+      </c>
+      <c r="I2" s="5">
+        <f>[1]Sheet1!J2</f>
+        <v>38.71</v>
+      </c>
+      <c r="J2" s="1">
+        <f>[1]Sheet1!K2</f>
+        <v>83</v>
       </c>
       <c r="K2" s="1">
-        <f>[1]Sheet1!$L2</f>
+        <f>[1]Sheet1!L2</f>
         <v>1013</v>
       </c>
       <c r="L2" s="1">
-        <f>[1]Sheet1!$M2</f>
-        <v>7</v>
+        <f>[1]Sheet1!M2</f>
+        <v>9.77</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="A3" s="1" t="str">
+        <f>[1]Sheet1!B3</f>
+        <v>09\09\24</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f>[1]Sheet1!C3</f>
+        <v>seg</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>[1]Sheet1!D3</f>
+        <v>14:27:06</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>[1]Sheet1!E3</f>
+        <v>Sobral</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>[1]Sheet1!F3</f>
+        <v>céu limpo</v>
+      </c>
+      <c r="F3" s="5">
+        <f>[1]Sheet1!G3</f>
+        <v>36.28</v>
+      </c>
+      <c r="G3" s="5">
+        <f>[1]Sheet1!H3</f>
+        <v>36.28</v>
+      </c>
+      <c r="H3" s="5">
+        <f>[1]Sheet1!I3</f>
+        <v>36.28</v>
+      </c>
+      <c r="I3" s="5">
+        <f>[1]Sheet1!J3</f>
+        <v>34.68</v>
+      </c>
+      <c r="J3" s="1">
+        <f>[1]Sheet1!K3</f>
+        <v>21</v>
+      </c>
+      <c r="K3" s="1">
+        <f>[1]Sheet1!L3</f>
+        <v>1011</v>
+      </c>
+      <c r="L3" s="1">
+        <f>[1]Sheet1!M3</f>
+        <v>3.85</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="A4" s="1" t="str">
+        <f>[1]Sheet1!B4</f>
+        <v>09\09\24</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f>[1]Sheet1!C4</f>
+        <v>seg</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>[1]Sheet1!D4</f>
+        <v>14:27:06</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>[1]Sheet1!E4</f>
+        <v>Acaraú</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f>[1]Sheet1!F4</f>
+        <v>céu limpo</v>
+      </c>
+      <c r="F4" s="5">
+        <f>[1]Sheet1!G4</f>
+        <v>30.77</v>
+      </c>
+      <c r="G4" s="5">
+        <f>[1]Sheet1!H4</f>
+        <v>30.77</v>
+      </c>
+      <c r="H4" s="5">
+        <f>[1]Sheet1!I4</f>
+        <v>30.77</v>
+      </c>
+      <c r="I4" s="5">
+        <f>[1]Sheet1!J4</f>
+        <v>32.43</v>
+      </c>
+      <c r="J4" s="1">
+        <f>[1]Sheet1!K4</f>
+        <v>51</v>
+      </c>
+      <c r="K4" s="1">
+        <f>[1]Sheet1!L4</f>
+        <v>1011</v>
+      </c>
+      <c r="L4" s="1">
+        <f>[1]Sheet1!M4</f>
+        <v>10.02</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="A5" s="1" t="str">
+        <f>[1]Sheet1!B5</f>
+        <v>09\09\24</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f>[1]Sheet1!C5</f>
+        <v>seg</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>[1]Sheet1!D5</f>
+        <v>14:27:06</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f>[1]Sheet1!E5</f>
+        <v>Itarema</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f>[1]Sheet1!F5</f>
+        <v>céu limpo</v>
+      </c>
+      <c r="F5" s="5">
+        <f>[1]Sheet1!G5</f>
+        <v>29.93</v>
+      </c>
+      <c r="G5" s="5">
+        <f>[1]Sheet1!H5</f>
+        <v>29.93</v>
+      </c>
+      <c r="H5" s="5">
+        <f>[1]Sheet1!I5</f>
+        <v>29.93</v>
+      </c>
+      <c r="I5" s="5">
+        <f>[1]Sheet1!J5</f>
+        <v>31.26</v>
+      </c>
+      <c r="J5" s="1">
+        <f>[1]Sheet1!K5</f>
+        <v>52</v>
+      </c>
+      <c r="K5" s="1">
+        <f>[1]Sheet1!L5</f>
+        <v>1012</v>
+      </c>
+      <c r="L5" s="1">
+        <f>[1]Sheet1!M5</f>
+        <v>9.6999999999999993</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -706,7 +2531,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="3"/>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
@@ -720,7 +2545,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="3"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
@@ -734,7 +2559,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="3"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
@@ -748,7 +2573,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
@@ -762,7 +2587,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="2"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
@@ -776,7 +2601,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
@@ -789,6 +2614,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B6F8FC-46A2-4B7D-900C-4C6F1498AB62}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6">
+        <v>30.77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="6">
+        <v>31.71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6">
+        <v>29.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6">
+        <v>36.28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6">
+        <v>32.172499999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5901B3E-A3E8-4B5E-9369-35A4919B8B84}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>